<commit_message>
Added Logout Page Test and code enhancement in exixting scripts
</commit_message>
<xml_diff>
--- a/MeritnationAutomation/Test Data/testData.xlsx
+++ b/MeritnationAutomation/Test Data/testData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="123">
   <si>
     <t>createAccountTest</t>
   </si>
@@ -37,7 +37,7 @@
     <t>9122970035</t>
   </si>
   <si>
-    <t>Delhi Public School</t>
+    <t>Meriton</t>
   </si>
   <si>
     <t>LoginTest</t>
@@ -103,60 +103,63 @@
     <t>BOARD EXAM PREPARATION</t>
   </si>
   <si>
-    <t>NEET</t>
+    <t>NEET (LIVE)</t>
+  </si>
+  <si>
+    <t>JEE (LIVE)</t>
+  </si>
+  <si>
+    <t>CLASS 12-COMMERCE</t>
+  </si>
+  <si>
+    <t>NEET CATALYST</t>
+  </si>
+  <si>
+    <t>IIT POWER PREP</t>
+  </si>
+  <si>
+    <t>VEDIC MATH</t>
+  </si>
+  <si>
+    <t>CBSE CLASS 6</t>
+  </si>
+  <si>
+    <t>CBSE CLASS 7</t>
+  </si>
+  <si>
+    <t>CBSE CLASS 8</t>
+  </si>
+  <si>
+    <t>CBSE CLASS 9</t>
+  </si>
+  <si>
+    <t>CBSE CLASS 10</t>
+  </si>
+  <si>
+    <t>12-SCIENCE</t>
+  </si>
+  <si>
+    <t>OLYMPIAD</t>
+  </si>
+  <si>
+    <t>11-SCIENCE</t>
+  </si>
+  <si>
+    <t>LIVE LITE CLASS 6</t>
+  </si>
+  <si>
+    <t>LIVE LITE CLASS 7</t>
+  </si>
+  <si>
+    <t>LIVE LITE CLASS 8</t>
+  </si>
+  <si>
+    <t>FOUNDATION (LIVE)</t>
   </si>
   <si>
     <t>JEE</t>
   </si>
   <si>
-    <t>CLASS 12-COMMERCE</t>
-  </si>
-  <si>
-    <t>NEET CATALYST</t>
-  </si>
-  <si>
-    <t>IIT POWER PREP</t>
-  </si>
-  <si>
-    <t>VEDIC MATH</t>
-  </si>
-  <si>
-    <t>CBSE CLASS 6</t>
-  </si>
-  <si>
-    <t>CBSE CLASS 7</t>
-  </si>
-  <si>
-    <t>CBSE CLASS 8</t>
-  </si>
-  <si>
-    <t>CBSE CLASS 9</t>
-  </si>
-  <si>
-    <t>CBSE CLASS 10</t>
-  </si>
-  <si>
-    <t>12-SCIENCE</t>
-  </si>
-  <si>
-    <t>OLYMPIAD</t>
-  </si>
-  <si>
-    <t>11-SCIENCE</t>
-  </si>
-  <si>
-    <t>LIVE LITE CLASS 6</t>
-  </si>
-  <si>
-    <t>LIVE LITE CLASS 7</t>
-  </si>
-  <si>
-    <t>LIVE LITE CLASS 8</t>
-  </si>
-  <si>
-    <t>FOUNDATION</t>
-  </si>
-  <si>
     <t>BBA</t>
   </si>
   <si>
@@ -172,13 +175,19 @@
     <t>ENGLISH GRAMMAR</t>
   </si>
   <si>
+    <t>BBA (LIVE)</t>
+  </si>
+  <si>
+    <t>CPT</t>
+  </si>
+  <si>
     <t>LIVE BOOSTER</t>
   </si>
   <si>
     <t>APPLIED GRAMMAR</t>
   </si>
   <si>
-    <t>CPT</t>
+    <t>BBA: CRASH COURSE</t>
   </si>
   <si>
     <t>LIVE LITE</t>
@@ -260,6 +269,9 @@
     <t>Aptitude Tests</t>
   </si>
   <si>
+    <t>Personality Tests</t>
+  </si>
+  <si>
     <t>Interest Test</t>
   </si>
   <si>
@@ -309,6 +321,72 @@
   </si>
   <si>
     <t>JEE Power Prep</t>
+  </si>
+  <si>
+    <t>CLASS 12(Science)</t>
+  </si>
+  <si>
+    <t>CLASS 12 (Commerce)</t>
+  </si>
+  <si>
+    <t>Board Paper solution</t>
+  </si>
+  <si>
+    <t>enggqatest+61@meritnation.com</t>
+  </si>
+  <si>
+    <t>LogoutTest</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/products/purchase</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/ncert-solutions</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/testprep</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/cbse-class-12-science/46</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/cbse-class-11-science/41</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/cbse-class-10/12</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/cbse-class-9/11</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/cbse-class-8/10</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/cbse-class-7/9</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/cbse-class-6/8</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/junior/grade-5</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/junior/grade-4</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/junior/grade-3</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/junior/grade-2</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/junior/grade-1</t>
+  </si>
+  <si>
+    <t>https://www.meritnation.com/live-new</t>
   </si>
 </sst>
 </file>
@@ -342,7 +420,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,6 +437,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF66"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -396,7 +486,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -427,6 +517,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -506,15 +608,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I50" activeCellId="0" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9676113360324"/>
     <col collapsed="false" hidden="false" max="8" min="2" style="0" width="8.66801619433198"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8056680161943"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.66801619433198"/>
@@ -737,7 +839,7 @@
         <v>45</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>45</v>
@@ -749,7 +851,7 @@
         <v>29</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>29</v>
@@ -773,16 +875,16 @@
         <v>40</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>28</v>
@@ -791,7 +893,7 @@
         <v>28</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>28</v>
@@ -803,16 +905,16 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>45</v>
@@ -821,114 +923,111 @@
         <v>40</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>40</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
-      <c r="B11" s="3" t="s">
-        <v>52</v>
+      <c r="B11" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="F12" s="3"/>
       <c r="H12" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>27</v>
@@ -947,7 +1046,7 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F13" s="3"/>
       <c r="H13" s="0" t="s">
@@ -973,7 +1072,7 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F14" s="3"/>
       <c r="J14" s="3"/>
@@ -991,755 +1090,933 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="M18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="N18" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="N35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="O35" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="36" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="L36" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="P36" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="M36" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="N36" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="O36" s="7" t="s">
-        <v>96</v>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1752,6 +2029,10 @@
     <hyperlink ref="M2" r:id="rId6" display="enggqatest+62@meritnation.com"/>
     <hyperlink ref="N2" r:id="rId7" display="enggqatest+93@meritnation.com"/>
     <hyperlink ref="O2" r:id="rId8" display="enggqatest+92@meritnation.com"/>
+    <hyperlink ref="B40" r:id="rId9" display="enggqatest+83@meritnation.com"/>
+    <hyperlink ref="C40" r:id="rId10" display="enggqatest+61@meritnation.com"/>
+    <hyperlink ref="D40" r:id="rId11" display="enggqatest+34@meritnation.com"/>
+    <hyperlink ref="B43" r:id="rId12" display="https://www.meritnation.com/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>